<commit_message>
index code 비교 갱신
</commit_message>
<xml_diff>
--- a/Doc/index code 비교 Daishin vs. Ebest.xlsx
+++ b/Doc/index code 비교 Daishin vs. Ebest.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="714">
   <si>
     <t>001</t>
   </si>
@@ -1544,6 +1544,630 @@
   <si>
     <t>Ebest</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>188</t>
+  </si>
+  <si>
+    <t>KOSTAR지수</t>
+  </si>
+  <si>
+    <t>189</t>
+  </si>
+  <si>
+    <t>KOSDAQ프리미어지수</t>
+  </si>
+  <si>
+    <t>(코스닥)종합</t>
+  </si>
+  <si>
+    <t>(코스닥)KOSDAQ 100</t>
+  </si>
+  <si>
+    <t>203</t>
+  </si>
+  <si>
+    <t>(코스닥)KOSDAQ MID 300</t>
+  </si>
+  <si>
+    <t>(코스닥)KOSDAQ SMALL</t>
+  </si>
+  <si>
+    <t>(코스닥)기타</t>
+  </si>
+  <si>
+    <t>(코스닥)IT종합</t>
+  </si>
+  <si>
+    <t>224</t>
+  </si>
+  <si>
+    <t>(코스닥)제조</t>
+  </si>
+  <si>
+    <t>226</t>
+  </si>
+  <si>
+    <t>(코스닥)건설</t>
+  </si>
+  <si>
+    <t>227</t>
+  </si>
+  <si>
+    <t>(코스닥)유통</t>
+  </si>
+  <si>
+    <t>229</t>
+  </si>
+  <si>
+    <t>(코스닥)운송</t>
+  </si>
+  <si>
+    <t>231</t>
+  </si>
+  <si>
+    <t>(코스닥)금융</t>
+  </si>
+  <si>
+    <t>237</t>
+  </si>
+  <si>
+    <t>(코스닥)오락, 문화</t>
+  </si>
+  <si>
+    <t>241</t>
+  </si>
+  <si>
+    <t>(코스닥)통신방송서비스</t>
+  </si>
+  <si>
+    <t>242</t>
+  </si>
+  <si>
+    <t>(코스닥)IT S/W &amp; SVC</t>
+  </si>
+  <si>
+    <t>243</t>
+  </si>
+  <si>
+    <t>(코스닥)IT H/W</t>
+  </si>
+  <si>
+    <t>256</t>
+  </si>
+  <si>
+    <t>(코스닥)음식료, 담배</t>
+  </si>
+  <si>
+    <t>258</t>
+  </si>
+  <si>
+    <t>(코스닥)섬유, 의류</t>
+  </si>
+  <si>
+    <t>262</t>
+  </si>
+  <si>
+    <t>(코스닥)종이, 목재</t>
+  </si>
+  <si>
+    <t>263</t>
+  </si>
+  <si>
+    <t>(코스닥)출판, 매체복제</t>
+  </si>
+  <si>
+    <t>265</t>
+  </si>
+  <si>
+    <t>(코스닥)화학</t>
+  </si>
+  <si>
+    <t>266</t>
+  </si>
+  <si>
+    <t>(코스닥)제약</t>
+  </si>
+  <si>
+    <t>267</t>
+  </si>
+  <si>
+    <t>(코스닥)비금속</t>
+  </si>
+  <si>
+    <t>268</t>
+  </si>
+  <si>
+    <t>(코스닥)금속</t>
+  </si>
+  <si>
+    <t>270</t>
+  </si>
+  <si>
+    <t>(코스닥)기계, 장비</t>
+  </si>
+  <si>
+    <t>272</t>
+  </si>
+  <si>
+    <t>(코스닥)일반전기전자</t>
+  </si>
+  <si>
+    <t>274</t>
+  </si>
+  <si>
+    <t>(코스닥)의료, 정밀기기</t>
+  </si>
+  <si>
+    <t>275</t>
+  </si>
+  <si>
+    <t>(코스닥)운송장비, 부품</t>
+  </si>
+  <si>
+    <t>277</t>
+  </si>
+  <si>
+    <t>(코스닥)기타 제조</t>
+  </si>
+  <si>
+    <t>351</t>
+  </si>
+  <si>
+    <t>(코스닥)통신서비스</t>
+  </si>
+  <si>
+    <t>352</t>
+  </si>
+  <si>
+    <t>(코스닥)방송서비스</t>
+  </si>
+  <si>
+    <t>353</t>
+  </si>
+  <si>
+    <t>(코스닥)인터넷</t>
+  </si>
+  <si>
+    <t>354</t>
+  </si>
+  <si>
+    <t>(코스닥)디지털컨텐츠</t>
+  </si>
+  <si>
+    <t>355</t>
+  </si>
+  <si>
+    <t>(코스닥)소프트웨어</t>
+  </si>
+  <si>
+    <t>356</t>
+  </si>
+  <si>
+    <t>(코스닥)컴퓨터서비스</t>
+  </si>
+  <si>
+    <t>357</t>
+  </si>
+  <si>
+    <t>(코스닥)통신장비</t>
+  </si>
+  <si>
+    <t>358</t>
+  </si>
+  <si>
+    <t>(코스닥)정보기기</t>
+  </si>
+  <si>
+    <t>359</t>
+  </si>
+  <si>
+    <t>(코스닥)반도체</t>
+  </si>
+  <si>
+    <t>360</t>
+  </si>
+  <si>
+    <t>(코스닥)IT부품</t>
+  </si>
+  <si>
+    <t>381</t>
+  </si>
+  <si>
+    <t>(코스닥)우량기업</t>
+  </si>
+  <si>
+    <t>382</t>
+  </si>
+  <si>
+    <t>(코스닥)벤처기업</t>
+  </si>
+  <si>
+    <t>383</t>
+  </si>
+  <si>
+    <t>(코스닥)중견기업</t>
+  </si>
+  <si>
+    <t>384</t>
+  </si>
+  <si>
+    <t>(코스닥)기술성장기업</t>
+  </si>
+  <si>
+    <t>390</t>
+  </si>
+  <si>
+    <t>코스닥 150</t>
+  </si>
+  <si>
+    <t>391</t>
+  </si>
+  <si>
+    <t>코스닥 150 동일가중지수</t>
+  </si>
+  <si>
+    <t>392</t>
+  </si>
+  <si>
+    <t>코스닥 150 레버리지지수</t>
+  </si>
+  <si>
+    <t>393</t>
+  </si>
+  <si>
+    <t>코스닥 150 선물지수</t>
+  </si>
+  <si>
+    <t>394</t>
+  </si>
+  <si>
+    <t>코스닥 150 선물 인버스지수</t>
+  </si>
+  <si>
+    <t>395</t>
+  </si>
+  <si>
+    <t>코스닥 150 선물 인버스-2X지수</t>
+  </si>
+  <si>
+    <t>396</t>
+  </si>
+  <si>
+    <t>코스닥 150 선물 인버스-3X지수</t>
+  </si>
+  <si>
+    <t>397</t>
+  </si>
+  <si>
+    <t>코스닥 150 레버리지 0.5지수</t>
+  </si>
+  <si>
+    <t>농업</t>
+  </si>
+  <si>
+    <t>임업</t>
+  </si>
+  <si>
+    <t>어업</t>
+  </si>
+  <si>
+    <t>석탄,원유및천연가스광업</t>
+  </si>
+  <si>
+    <t>금속광업</t>
+  </si>
+  <si>
+    <t>비금속광물광업</t>
+  </si>
+  <si>
+    <t>광업지원서비스업</t>
+  </si>
+  <si>
+    <t>610</t>
+  </si>
+  <si>
+    <t>식료품제조업</t>
+  </si>
+  <si>
+    <t>611</t>
+  </si>
+  <si>
+    <t>음료제조업</t>
+  </si>
+  <si>
+    <t>612</t>
+  </si>
+  <si>
+    <t>담배제조업</t>
+  </si>
+  <si>
+    <t>613</t>
+  </si>
+  <si>
+    <t>섬유제품제조업</t>
+  </si>
+  <si>
+    <t>614</t>
+  </si>
+  <si>
+    <t>의복,의복액세서리및모피제품제조업</t>
+  </si>
+  <si>
+    <t>가죽,가방및신발제조업</t>
+  </si>
+  <si>
+    <t>목재및나무제품제조업</t>
+  </si>
+  <si>
+    <t>펄프,종이및종이제품제조업</t>
+  </si>
+  <si>
+    <t>인쇄및기록매체복제업</t>
+  </si>
+  <si>
+    <t>코크스,연탄및석유정제품제조업</t>
+  </si>
+  <si>
+    <t>화학물질및화학제품제조업</t>
+  </si>
+  <si>
+    <t>의료용물질및의약품제조업</t>
+  </si>
+  <si>
+    <t>고무제품및플라스틱제품제조업</t>
+  </si>
+  <si>
+    <t>비금속광물제품제조업</t>
+  </si>
+  <si>
+    <t>1차금속제조업</t>
+  </si>
+  <si>
+    <t>금속가공제품제조업</t>
+  </si>
+  <si>
+    <t>전자부품,컴퓨터,영상,음향및통신장비제조업</t>
+  </si>
+  <si>
+    <t>의료,정밀,광학기기및시계제조업</t>
+  </si>
+  <si>
+    <t>전기장비제조업</t>
+  </si>
+  <si>
+    <t>기타기계및장비제조업</t>
+  </si>
+  <si>
+    <t>자동차및트레일러제조업</t>
+  </si>
+  <si>
+    <t>기타운송장비제조업</t>
+  </si>
+  <si>
+    <t>가구제조업</t>
+  </si>
+  <si>
+    <t>기타제품제조업</t>
+  </si>
+  <si>
+    <t>전기,가스,증기및공기조절공급업</t>
+  </si>
+  <si>
+    <t>수도사업</t>
+  </si>
+  <si>
+    <t>하수,폐수및분뇨처리업</t>
+  </si>
+  <si>
+    <t>폐기물수집운반,처리및원료재생업</t>
+  </si>
+  <si>
+    <t>환경정화및복원업</t>
+  </si>
+  <si>
+    <t>종합건설업</t>
+  </si>
+  <si>
+    <t>전문직별공사업</t>
+  </si>
+  <si>
+    <t>자동차및부품판매업</t>
+  </si>
+  <si>
+    <t>도매및상품중개업</t>
+  </si>
+  <si>
+    <t>소매업</t>
+  </si>
+  <si>
+    <t>육상운송및파이프라인운송업</t>
+  </si>
+  <si>
+    <t>수상운송업</t>
+  </si>
+  <si>
+    <t>항공운송업</t>
+  </si>
+  <si>
+    <t>창고및운송관련서비스업</t>
+  </si>
+  <si>
+    <t>숙박업</t>
+  </si>
+  <si>
+    <t>656</t>
+  </si>
+  <si>
+    <t>음식점및주점업</t>
+  </si>
+  <si>
+    <t>658</t>
+  </si>
+  <si>
+    <t>출판업</t>
+  </si>
+  <si>
+    <t>659</t>
+  </si>
+  <si>
+    <t>영상·오디오기록물제작및배급업</t>
+  </si>
+  <si>
+    <t>660</t>
+  </si>
+  <si>
+    <t>방송업</t>
+  </si>
+  <si>
+    <t>661</t>
+  </si>
+  <si>
+    <t>662</t>
+  </si>
+  <si>
+    <t>컴퓨터프로그래밍,시스템통합및관리업</t>
+  </si>
+  <si>
+    <t>663</t>
+  </si>
+  <si>
+    <t>정보서비스업</t>
+  </si>
+  <si>
+    <t>664</t>
+  </si>
+  <si>
+    <t>665</t>
+  </si>
+  <si>
+    <t>보험및연금업</t>
+  </si>
+  <si>
+    <t>666</t>
+  </si>
+  <si>
+    <t>금융및보험관련서비스업</t>
+  </si>
+  <si>
+    <t>668</t>
+  </si>
+  <si>
+    <t>부동산업</t>
+  </si>
+  <si>
+    <t>669</t>
+  </si>
+  <si>
+    <t>임대업</t>
+  </si>
+  <si>
+    <t>670</t>
+  </si>
+  <si>
+    <t>연구개발업</t>
+  </si>
+  <si>
+    <t>671</t>
+  </si>
+  <si>
+    <t>전문서비스업</t>
+  </si>
+  <si>
+    <t>672</t>
+  </si>
+  <si>
+    <t>건축기술,엔지니어링및기타과학기술서비스업</t>
+  </si>
+  <si>
+    <t>673</t>
+  </si>
+  <si>
+    <t>기타전문,과학및기술서비스업</t>
+  </si>
+  <si>
+    <t>674</t>
+  </si>
+  <si>
+    <t>사업시설관리및조경서비스업</t>
+  </si>
+  <si>
+    <t>675</t>
+  </si>
+  <si>
+    <t>사업지원서비스업</t>
+  </si>
+  <si>
+    <t>684</t>
+  </si>
+  <si>
+    <t>공공행정,국방및사회보장행정</t>
+  </si>
+  <si>
+    <t>685</t>
+  </si>
+  <si>
+    <t>교육서비스업</t>
+  </si>
+  <si>
+    <t>686</t>
+  </si>
+  <si>
+    <t>보건업</t>
+  </si>
+  <si>
+    <t>687</t>
+  </si>
+  <si>
+    <t>사회복지서비스업</t>
+  </si>
+  <si>
+    <t>690</t>
+  </si>
+  <si>
+    <t>창작,예술및여가관련서비스업</t>
+  </si>
+  <si>
+    <t>691</t>
+  </si>
+  <si>
+    <t>스포츠및오락관련서비스업</t>
+  </si>
+  <si>
+    <t>694</t>
+  </si>
+  <si>
+    <t>협회및단체</t>
+  </si>
+  <si>
+    <t>695</t>
+  </si>
+  <si>
+    <t>수리업</t>
+  </si>
+  <si>
+    <t>696</t>
+  </si>
+  <si>
+    <t>기타개인서비스업</t>
+  </si>
+  <si>
+    <t>697</t>
+  </si>
+  <si>
+    <t>가구내고용활동</t>
+  </si>
+  <si>
+    <t>698</t>
+  </si>
+  <si>
+    <t>자가소비를위한가구의재화및서비스생산활동</t>
+  </si>
+  <si>
+    <t>699</t>
+  </si>
+  <si>
+    <t>(K-OTC)K-OTC 관련</t>
   </si>
 </sst>
 </file>
@@ -1873,10 +2497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F172"/>
+  <dimension ref="A1:F227"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
+      <selection activeCell="L220" sqref="L220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2689,10 +3313,10 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>114</v>
+        <v>506</v>
       </c>
       <c r="B59" t="s">
-        <v>115</v>
+        <v>507</v>
       </c>
       <c r="E59" t="s">
         <v>397</v>
@@ -2703,10 +3327,10 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>116</v>
+        <v>508</v>
       </c>
       <c r="B60" t="s">
-        <v>117</v>
+        <v>509</v>
       </c>
       <c r="E60" t="s">
         <v>398</v>
@@ -2717,10 +3341,10 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B61" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E61" t="s">
         <v>399</v>
@@ -2731,10 +3355,10 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B62" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E62" t="s">
         <v>400</v>
@@ -2745,10 +3369,10 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B63" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E63" t="s">
         <v>401</v>
@@ -2759,10 +3383,10 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B64" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E64" t="s">
         <v>402</v>
@@ -2773,10 +3397,10 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B65" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E65" t="s">
         <v>403</v>
@@ -2787,10 +3411,10 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B66" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E66" t="s">
         <v>404</v>
@@ -2801,10 +3425,10 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>130</v>
+        <v>378</v>
       </c>
       <c r="B67" t="s">
-        <v>131</v>
+        <v>510</v>
       </c>
       <c r="E67" t="s">
         <v>405</v>
@@ -2815,10 +3439,10 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>132</v>
+        <v>379</v>
       </c>
       <c r="B68" t="s">
-        <v>133</v>
+        <v>511</v>
       </c>
       <c r="E68" t="s">
         <v>406</v>
@@ -2829,10 +3453,10 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>134</v>
+        <v>512</v>
       </c>
       <c r="B69" t="s">
-        <v>135</v>
+        <v>513</v>
       </c>
       <c r="E69" t="s">
         <v>407</v>
@@ -2843,10 +3467,10 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>136</v>
+        <v>380</v>
       </c>
       <c r="B70" t="s">
-        <v>137</v>
+        <v>514</v>
       </c>
       <c r="E70" t="s">
         <v>408</v>
@@ -2857,10 +3481,10 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>138</v>
+        <v>388</v>
       </c>
       <c r="B71" t="s">
-        <v>139</v>
+        <v>515</v>
       </c>
       <c r="E71" t="s">
         <v>409</v>
@@ -2871,10 +3495,10 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>140</v>
+        <v>391</v>
       </c>
       <c r="B72" t="s">
-        <v>141</v>
+        <v>516</v>
       </c>
       <c r="E72" t="s">
         <v>410</v>
@@ -2885,10 +3509,10 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>142</v>
+        <v>517</v>
       </c>
       <c r="B73" t="s">
-        <v>143</v>
+        <v>518</v>
       </c>
       <c r="E73" t="s">
         <v>411</v>
@@ -2899,10 +3523,10 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>144</v>
+        <v>519</v>
       </c>
       <c r="B74" t="s">
-        <v>145</v>
+        <v>520</v>
       </c>
       <c r="E74" t="s">
         <v>412</v>
@@ -2913,10 +3537,10 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>146</v>
+        <v>521</v>
       </c>
       <c r="B75" t="s">
-        <v>147</v>
+        <v>522</v>
       </c>
       <c r="E75" t="s">
         <v>413</v>
@@ -2927,10 +3551,10 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>148</v>
+        <v>523</v>
       </c>
       <c r="B76" t="s">
-        <v>149</v>
+        <v>524</v>
       </c>
       <c r="E76" t="s">
         <v>414</v>
@@ -2941,10 +3565,10 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>150</v>
+        <v>525</v>
       </c>
       <c r="B77" t="s">
-        <v>151</v>
+        <v>526</v>
       </c>
       <c r="E77" t="s">
         <v>415</v>
@@ -2955,10 +3579,10 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>152</v>
+        <v>527</v>
       </c>
       <c r="B78" t="s">
-        <v>153</v>
+        <v>528</v>
       </c>
       <c r="E78" t="s">
         <v>416</v>
@@ -2969,10 +3593,10 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>154</v>
+        <v>529</v>
       </c>
       <c r="B79" t="s">
-        <v>155</v>
+        <v>530</v>
       </c>
       <c r="E79" t="s">
         <v>417</v>
@@ -2983,10 +3607,10 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>156</v>
+        <v>531</v>
       </c>
       <c r="B80" t="s">
-        <v>157</v>
+        <v>532</v>
       </c>
       <c r="E80" t="s">
         <v>418</v>
@@ -2997,10 +3621,10 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>158</v>
+        <v>533</v>
       </c>
       <c r="B81" t="s">
-        <v>159</v>
+        <v>534</v>
       </c>
       <c r="E81" t="s">
         <v>419</v>
@@ -3011,10 +3635,10 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>160</v>
+        <v>535</v>
       </c>
       <c r="B82" t="s">
-        <v>161</v>
+        <v>536</v>
       </c>
       <c r="E82" t="s">
         <v>420</v>
@@ -3025,10 +3649,10 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>162</v>
+        <v>537</v>
       </c>
       <c r="B83" t="s">
-        <v>163</v>
+        <v>538</v>
       </c>
       <c r="E83" t="s">
         <v>421</v>
@@ -3039,10 +3663,10 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>164</v>
+        <v>539</v>
       </c>
       <c r="B84" t="s">
-        <v>165</v>
+        <v>540</v>
       </c>
       <c r="E84" t="s">
         <v>422</v>
@@ -3053,10 +3677,10 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>166</v>
+        <v>541</v>
       </c>
       <c r="B85" t="s">
-        <v>167</v>
+        <v>542</v>
       </c>
       <c r="E85" t="s">
         <v>423</v>
@@ -3067,10 +3691,10 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>168</v>
+        <v>543</v>
       </c>
       <c r="B86" t="s">
-        <v>169</v>
+        <v>544</v>
       </c>
       <c r="E86" t="s">
         <v>424</v>
@@ -3081,10 +3705,10 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>170</v>
+        <v>545</v>
       </c>
       <c r="B87" t="s">
-        <v>171</v>
+        <v>546</v>
       </c>
       <c r="E87" t="s">
         <v>425</v>
@@ -3095,10 +3719,10 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>172</v>
+        <v>547</v>
       </c>
       <c r="B88" t="s">
-        <v>173</v>
+        <v>548</v>
       </c>
       <c r="E88" t="s">
         <v>426</v>
@@ -3109,10 +3733,10 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>174</v>
+        <v>549</v>
       </c>
       <c r="B89" t="s">
-        <v>175</v>
+        <v>550</v>
       </c>
       <c r="E89" t="s">
         <v>427</v>
@@ -3123,10 +3747,10 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>176</v>
+        <v>551</v>
       </c>
       <c r="B90" t="s">
-        <v>177</v>
+        <v>552</v>
       </c>
       <c r="E90" t="s">
         <v>428</v>
@@ -3137,10 +3761,10 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>178</v>
+        <v>553</v>
       </c>
       <c r="B91" t="s">
-        <v>179</v>
+        <v>554</v>
       </c>
       <c r="E91" t="s">
         <v>429</v>
@@ -3151,10 +3775,10 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>180</v>
+        <v>555</v>
       </c>
       <c r="B92" t="s">
-        <v>181</v>
+        <v>556</v>
       </c>
       <c r="E92" t="s">
         <v>430</v>
@@ -3165,10 +3789,10 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>182</v>
+        <v>557</v>
       </c>
       <c r="B93" t="s">
-        <v>183</v>
+        <v>558</v>
       </c>
       <c r="E93" t="s">
         <v>431</v>
@@ -3179,10 +3803,10 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>184</v>
+        <v>559</v>
       </c>
       <c r="B94" t="s">
-        <v>185</v>
+        <v>560</v>
       </c>
       <c r="E94" t="s">
         <v>432</v>
@@ -3193,10 +3817,10 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>186</v>
+        <v>561</v>
       </c>
       <c r="B95" t="s">
-        <v>187</v>
+        <v>562</v>
       </c>
       <c r="E95" t="s">
         <v>433</v>
@@ -3207,10 +3831,10 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>188</v>
+        <v>563</v>
       </c>
       <c r="B96" t="s">
-        <v>189</v>
+        <v>564</v>
       </c>
       <c r="E96" t="s">
         <v>434</v>
@@ -3221,10 +3845,10 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>190</v>
+        <v>565</v>
       </c>
       <c r="B97" t="s">
-        <v>191</v>
+        <v>566</v>
       </c>
       <c r="E97" t="s">
         <v>435</v>
@@ -3235,10 +3859,10 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>192</v>
+        <v>567</v>
       </c>
       <c r="B98" t="s">
-        <v>193</v>
+        <v>568</v>
       </c>
       <c r="E98" t="s">
         <v>436</v>
@@ -3249,10 +3873,10 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>194</v>
+        <v>569</v>
       </c>
       <c r="B99" t="s">
-        <v>195</v>
+        <v>570</v>
       </c>
       <c r="E99" t="s">
         <v>437</v>
@@ -3262,6 +3886,12 @@
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>571</v>
+      </c>
+      <c r="B100" t="s">
+        <v>572</v>
+      </c>
       <c r="E100" t="s">
         <v>438</v>
       </c>
@@ -3270,6 +3900,12 @@
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>573</v>
+      </c>
+      <c r="B101" t="s">
+        <v>574</v>
+      </c>
       <c r="E101" t="s">
         <v>439</v>
       </c>
@@ -3278,6 +3914,12 @@
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>575</v>
+      </c>
+      <c r="B102" t="s">
+        <v>576</v>
+      </c>
       <c r="E102" t="s">
         <v>440</v>
       </c>
@@ -3286,6 +3928,12 @@
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>577</v>
+      </c>
+      <c r="B103" t="s">
+        <v>578</v>
+      </c>
       <c r="E103" t="s">
         <v>441</v>
       </c>
@@ -3294,6 +3942,12 @@
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>579</v>
+      </c>
+      <c r="B104" t="s">
+        <v>580</v>
+      </c>
       <c r="E104" t="s">
         <v>126</v>
       </c>
@@ -3302,6 +3956,12 @@
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>581</v>
+      </c>
+      <c r="B105" t="s">
+        <v>582</v>
+      </c>
       <c r="E105" t="s">
         <v>128</v>
       </c>
@@ -3310,6 +3970,12 @@
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>583</v>
+      </c>
+      <c r="B106" t="s">
+        <v>584</v>
+      </c>
       <c r="E106" t="s">
         <v>130</v>
       </c>
@@ -3318,6 +3984,12 @@
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>585</v>
+      </c>
+      <c r="B107" t="s">
+        <v>586</v>
+      </c>
       <c r="E107" t="s">
         <v>132</v>
       </c>
@@ -3326,6 +3998,12 @@
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>587</v>
+      </c>
+      <c r="B108" t="s">
+        <v>588</v>
+      </c>
       <c r="E108" t="s">
         <v>442</v>
       </c>
@@ -3334,6 +4012,12 @@
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>589</v>
+      </c>
+      <c r="B109" t="s">
+        <v>590</v>
+      </c>
       <c r="E109" t="s">
         <v>443</v>
       </c>
@@ -3342,6 +4026,12 @@
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>591</v>
+      </c>
+      <c r="B110" t="s">
+        <v>592</v>
+      </c>
       <c r="E110" t="s">
         <v>444</v>
       </c>
@@ -3350,6 +4040,12 @@
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>593</v>
+      </c>
+      <c r="B111" t="s">
+        <v>594</v>
+      </c>
       <c r="E111" t="s">
         <v>445</v>
       </c>
@@ -3358,6 +4054,12 @@
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>595</v>
+      </c>
+      <c r="B112" t="s">
+        <v>596</v>
+      </c>
       <c r="E112" t="s">
         <v>134</v>
       </c>
@@ -3365,7 +4067,13 @@
         <v>305</v>
       </c>
     </row>
-    <row r="113" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>597</v>
+      </c>
+      <c r="B113" t="s">
+        <v>598</v>
+      </c>
       <c r="E113" t="s">
         <v>138</v>
       </c>
@@ -3373,7 +4081,13 @@
         <v>306</v>
       </c>
     </row>
-    <row r="114" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>599</v>
+      </c>
+      <c r="B114" t="s">
+        <v>600</v>
+      </c>
       <c r="E114" t="s">
         <v>140</v>
       </c>
@@ -3381,7 +4095,13 @@
         <v>307</v>
       </c>
     </row>
-    <row r="115" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>601</v>
+      </c>
+      <c r="B115" t="s">
+        <v>602</v>
+      </c>
       <c r="E115" t="s">
         <v>446</v>
       </c>
@@ -3389,7 +4109,13 @@
         <v>308</v>
       </c>
     </row>
-    <row r="116" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>603</v>
+      </c>
+      <c r="B116" t="s">
+        <v>604</v>
+      </c>
       <c r="E116" t="s">
         <v>447</v>
       </c>
@@ -3397,7 +4123,13 @@
         <v>309</v>
       </c>
     </row>
-    <row r="117" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>126</v>
+      </c>
+      <c r="B117" t="s">
+        <v>127</v>
+      </c>
       <c r="E117" t="s">
         <v>448</v>
       </c>
@@ -3405,7 +4137,13 @@
         <v>310</v>
       </c>
     </row>
-    <row r="118" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>128</v>
+      </c>
+      <c r="B118" t="s">
+        <v>129</v>
+      </c>
       <c r="E118" t="s">
         <v>449</v>
       </c>
@@ -3413,7 +4151,13 @@
         <v>311</v>
       </c>
     </row>
-    <row r="119" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>130</v>
+      </c>
+      <c r="B119" t="s">
+        <v>131</v>
+      </c>
       <c r="E119" t="s">
         <v>450</v>
       </c>
@@ -3421,7 +4165,13 @@
         <v>312</v>
       </c>
     </row>
-    <row r="120" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>132</v>
+      </c>
+      <c r="B120" t="s">
+        <v>133</v>
+      </c>
       <c r="E120" t="s">
         <v>451</v>
       </c>
@@ -3429,7 +4179,13 @@
         <v>313</v>
       </c>
     </row>
-    <row r="121" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>134</v>
+      </c>
+      <c r="B121" t="s">
+        <v>135</v>
+      </c>
       <c r="E121" t="s">
         <v>452</v>
       </c>
@@ -3437,7 +4193,13 @@
         <v>314</v>
       </c>
     </row>
-    <row r="122" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>136</v>
+      </c>
+      <c r="B122" t="s">
+        <v>137</v>
+      </c>
       <c r="E122" t="s">
         <v>453</v>
       </c>
@@ -3445,7 +4207,13 @@
         <v>315</v>
       </c>
     </row>
-    <row r="123" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>138</v>
+      </c>
+      <c r="B123" t="s">
+        <v>139</v>
+      </c>
       <c r="E123" t="s">
         <v>454</v>
       </c>
@@ -3453,7 +4221,13 @@
         <v>316</v>
       </c>
     </row>
-    <row r="124" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>140</v>
+      </c>
+      <c r="B124" t="s">
+        <v>141</v>
+      </c>
       <c r="E124" t="s">
         <v>455</v>
       </c>
@@ -3461,7 +4235,13 @@
         <v>317</v>
       </c>
     </row>
-    <row r="125" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>142</v>
+      </c>
+      <c r="B125" t="s">
+        <v>143</v>
+      </c>
       <c r="E125" t="s">
         <v>456</v>
       </c>
@@ -3469,7 +4249,13 @@
         <v>318</v>
       </c>
     </row>
-    <row r="126" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>144</v>
+      </c>
+      <c r="B126" t="s">
+        <v>145</v>
+      </c>
       <c r="E126" t="s">
         <v>457</v>
       </c>
@@ -3477,7 +4263,13 @@
         <v>319</v>
       </c>
     </row>
-    <row r="127" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>146</v>
+      </c>
+      <c r="B127" t="s">
+        <v>147</v>
+      </c>
       <c r="E127" t="s">
         <v>458</v>
       </c>
@@ -3485,7 +4277,13 @@
         <v>320</v>
       </c>
     </row>
-    <row r="128" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>148</v>
+      </c>
+      <c r="B128" t="s">
+        <v>149</v>
+      </c>
       <c r="E128" t="s">
         <v>459</v>
       </c>
@@ -3493,7 +4291,13 @@
         <v>321</v>
       </c>
     </row>
-    <row r="129" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>150</v>
+      </c>
+      <c r="B129" t="s">
+        <v>151</v>
+      </c>
       <c r="E129" t="s">
         <v>460</v>
       </c>
@@ -3501,7 +4305,13 @@
         <v>322</v>
       </c>
     </row>
-    <row r="130" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>152</v>
+      </c>
+      <c r="B130" t="s">
+        <v>153</v>
+      </c>
       <c r="E130" t="s">
         <v>461</v>
       </c>
@@ -3509,7 +4319,13 @@
         <v>323</v>
       </c>
     </row>
-    <row r="131" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>154</v>
+      </c>
+      <c r="B131" t="s">
+        <v>155</v>
+      </c>
       <c r="E131" t="s">
         <v>462</v>
       </c>
@@ -3517,7 +4333,13 @@
         <v>324</v>
       </c>
     </row>
-    <row r="132" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>156</v>
+      </c>
+      <c r="B132" t="s">
+        <v>157</v>
+      </c>
       <c r="E132" t="s">
         <v>463</v>
       </c>
@@ -3525,7 +4347,13 @@
         <v>325</v>
       </c>
     </row>
-    <row r="133" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>158</v>
+      </c>
+      <c r="B133" t="s">
+        <v>159</v>
+      </c>
       <c r="E133" t="s">
         <v>464</v>
       </c>
@@ -3533,7 +4361,13 @@
         <v>326</v>
       </c>
     </row>
-    <row r="134" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>160</v>
+      </c>
+      <c r="B134" t="s">
+        <v>161</v>
+      </c>
       <c r="E134" t="s">
         <v>465</v>
       </c>
@@ -3541,7 +4375,13 @@
         <v>327</v>
       </c>
     </row>
-    <row r="135" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>162</v>
+      </c>
+      <c r="B135" t="s">
+        <v>163</v>
+      </c>
       <c r="E135" t="s">
         <v>466</v>
       </c>
@@ -3549,7 +4389,13 @@
         <v>328</v>
       </c>
     </row>
-    <row r="136" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>164</v>
+      </c>
+      <c r="B136" t="s">
+        <v>165</v>
+      </c>
       <c r="E136" t="s">
         <v>467</v>
       </c>
@@ -3557,7 +4403,13 @@
         <v>329</v>
       </c>
     </row>
-    <row r="137" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>166</v>
+      </c>
+      <c r="B137" t="s">
+        <v>167</v>
+      </c>
       <c r="E137" t="s">
         <v>468</v>
       </c>
@@ -3565,7 +4417,13 @@
         <v>330</v>
       </c>
     </row>
-    <row r="138" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>168</v>
+      </c>
+      <c r="B138" t="s">
+        <v>169</v>
+      </c>
       <c r="E138" t="s">
         <v>469</v>
       </c>
@@ -3573,7 +4431,13 @@
         <v>331</v>
       </c>
     </row>
-    <row r="139" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>170</v>
+      </c>
+      <c r="B139" t="s">
+        <v>171</v>
+      </c>
       <c r="E139" t="s">
         <v>470</v>
       </c>
@@ -3581,7 +4445,13 @@
         <v>332</v>
       </c>
     </row>
-    <row r="140" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>172</v>
+      </c>
+      <c r="B140" t="s">
+        <v>173</v>
+      </c>
       <c r="E140" t="s">
         <v>471</v>
       </c>
@@ -3589,7 +4459,13 @@
         <v>333</v>
       </c>
     </row>
-    <row r="141" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>174</v>
+      </c>
+      <c r="B141" t="s">
+        <v>175</v>
+      </c>
       <c r="E141" t="s">
         <v>472</v>
       </c>
@@ -3597,7 +4473,13 @@
         <v>334</v>
       </c>
     </row>
-    <row r="142" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>176</v>
+      </c>
+      <c r="B142" t="s">
+        <v>177</v>
+      </c>
       <c r="E142" t="s">
         <v>473</v>
       </c>
@@ -3605,7 +4487,13 @@
         <v>335</v>
       </c>
     </row>
-    <row r="143" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>178</v>
+      </c>
+      <c r="B143" t="s">
+        <v>179</v>
+      </c>
       <c r="E143" t="s">
         <v>474</v>
       </c>
@@ -3613,7 +4501,13 @@
         <v>336</v>
       </c>
     </row>
-    <row r="144" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>180</v>
+      </c>
+      <c r="B144" t="s">
+        <v>181</v>
+      </c>
       <c r="E144" t="s">
         <v>475</v>
       </c>
@@ -3621,7 +4515,13 @@
         <v>337</v>
       </c>
     </row>
-    <row r="145" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>182</v>
+      </c>
+      <c r="B145" t="s">
+        <v>183</v>
+      </c>
       <c r="E145" t="s">
         <v>476</v>
       </c>
@@ -3629,7 +4529,13 @@
         <v>338</v>
       </c>
     </row>
-    <row r="146" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>184</v>
+      </c>
+      <c r="B146" t="s">
+        <v>185</v>
+      </c>
       <c r="E146" t="s">
         <v>477</v>
       </c>
@@ -3637,7 +4543,13 @@
         <v>339</v>
       </c>
     </row>
-    <row r="147" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>186</v>
+      </c>
+      <c r="B147" t="s">
+        <v>187</v>
+      </c>
       <c r="E147" t="s">
         <v>478</v>
       </c>
@@ -3645,7 +4557,13 @@
         <v>340</v>
       </c>
     </row>
-    <row r="148" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>188</v>
+      </c>
+      <c r="B148" t="s">
+        <v>189</v>
+      </c>
       <c r="E148" t="s">
         <v>479</v>
       </c>
@@ -3653,7 +4571,13 @@
         <v>341</v>
       </c>
     </row>
-    <row r="149" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>190</v>
+      </c>
+      <c r="B149" t="s">
+        <v>191</v>
+      </c>
       <c r="E149" t="s">
         <v>480</v>
       </c>
@@ -3661,7 +4585,13 @@
         <v>342</v>
       </c>
     </row>
-    <row r="150" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>192</v>
+      </c>
+      <c r="B150" t="s">
+        <v>193</v>
+      </c>
       <c r="E150" t="s">
         <v>481</v>
       </c>
@@ -3669,7 +4599,13 @@
         <v>343</v>
       </c>
     </row>
-    <row r="151" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>194</v>
+      </c>
+      <c r="B151" t="s">
+        <v>195</v>
+      </c>
       <c r="E151" t="s">
         <v>482</v>
       </c>
@@ -3677,7 +4613,13 @@
         <v>344</v>
       </c>
     </row>
-    <row r="152" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>454</v>
+      </c>
+      <c r="B152" t="s">
+        <v>605</v>
+      </c>
       <c r="E152" t="s">
         <v>483</v>
       </c>
@@ -3685,7 +4627,13 @@
         <v>345</v>
       </c>
     </row>
-    <row r="153" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>455</v>
+      </c>
+      <c r="B153" t="s">
+        <v>606</v>
+      </c>
       <c r="E153" t="s">
         <v>484</v>
       </c>
@@ -3693,7 +4641,13 @@
         <v>346</v>
       </c>
     </row>
-    <row r="154" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>456</v>
+      </c>
+      <c r="B154" t="s">
+        <v>607</v>
+      </c>
       <c r="E154" t="s">
         <v>485</v>
       </c>
@@ -3701,7 +4655,13 @@
         <v>347</v>
       </c>
     </row>
-    <row r="155" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>458</v>
+      </c>
+      <c r="B155" t="s">
+        <v>608</v>
+      </c>
       <c r="E155" t="s">
         <v>486</v>
       </c>
@@ -3709,7 +4669,13 @@
         <v>348</v>
       </c>
     </row>
-    <row r="156" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>459</v>
+      </c>
+      <c r="B156" t="s">
+        <v>609</v>
+      </c>
       <c r="E156" t="s">
         <v>487</v>
       </c>
@@ -3717,7 +4683,13 @@
         <v>349</v>
       </c>
     </row>
-    <row r="157" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>460</v>
+      </c>
+      <c r="B157" t="s">
+        <v>610</v>
+      </c>
       <c r="E157" t="s">
         <v>488</v>
       </c>
@@ -3725,7 +4697,13 @@
         <v>350</v>
       </c>
     </row>
-    <row r="158" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>461</v>
+      </c>
+      <c r="B158" t="s">
+        <v>611</v>
+      </c>
       <c r="E158" t="s">
         <v>489</v>
       </c>
@@ -3733,7 +4711,13 @@
         <v>351</v>
       </c>
     </row>
-    <row r="159" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>612</v>
+      </c>
+      <c r="B159" t="s">
+        <v>613</v>
+      </c>
       <c r="E159" t="s">
         <v>490</v>
       </c>
@@ -3741,7 +4725,13 @@
         <v>352</v>
       </c>
     </row>
-    <row r="160" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>614</v>
+      </c>
+      <c r="B160" t="s">
+        <v>615</v>
+      </c>
       <c r="E160" t="s">
         <v>491</v>
       </c>
@@ -3749,7 +4739,13 @@
         <v>353</v>
       </c>
     </row>
-    <row r="161" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>616</v>
+      </c>
+      <c r="B161" t="s">
+        <v>617</v>
+      </c>
       <c r="E161" t="s">
         <v>492</v>
       </c>
@@ -3757,7 +4753,13 @@
         <v>354</v>
       </c>
     </row>
-    <row r="162" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>618</v>
+      </c>
+      <c r="B162" t="s">
+        <v>619</v>
+      </c>
       <c r="E162" t="s">
         <v>493</v>
       </c>
@@ -3765,7 +4767,13 @@
         <v>355</v>
       </c>
     </row>
-    <row r="163" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>620</v>
+      </c>
+      <c r="B163" t="s">
+        <v>621</v>
+      </c>
       <c r="E163" t="s">
         <v>494</v>
       </c>
@@ -3773,7 +4781,13 @@
         <v>356</v>
       </c>
     </row>
-    <row r="164" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>463</v>
+      </c>
+      <c r="B164" t="s">
+        <v>622</v>
+      </c>
       <c r="E164" t="s">
         <v>495</v>
       </c>
@@ -3781,7 +4795,13 @@
         <v>357</v>
       </c>
     </row>
-    <row r="165" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>464</v>
+      </c>
+      <c r="B165" t="s">
+        <v>623</v>
+      </c>
       <c r="E165" t="s">
         <v>496</v>
       </c>
@@ -3789,7 +4809,13 @@
         <v>358</v>
       </c>
     </row>
-    <row r="166" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>465</v>
+      </c>
+      <c r="B166" t="s">
+        <v>624</v>
+      </c>
       <c r="E166" t="s">
         <v>497</v>
       </c>
@@ -3797,7 +4823,13 @@
         <v>359</v>
       </c>
     </row>
-    <row r="167" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>466</v>
+      </c>
+      <c r="B167" t="s">
+        <v>625</v>
+      </c>
       <c r="E167" t="s">
         <v>498</v>
       </c>
@@ -3805,7 +4837,13 @@
         <v>360</v>
       </c>
     </row>
-    <row r="168" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>467</v>
+      </c>
+      <c r="B168" t="s">
+        <v>626</v>
+      </c>
       <c r="E168" t="s">
         <v>499</v>
       </c>
@@ -3813,7 +4851,13 @@
         <v>361</v>
       </c>
     </row>
-    <row r="169" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>468</v>
+      </c>
+      <c r="B169" t="s">
+        <v>627</v>
+      </c>
       <c r="E169" t="s">
         <v>500</v>
       </c>
@@ -3821,7 +4865,13 @@
         <v>362</v>
       </c>
     </row>
-    <row r="170" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>469</v>
+      </c>
+      <c r="B170" t="s">
+        <v>628</v>
+      </c>
       <c r="E170" t="s">
         <v>501</v>
       </c>
@@ -3829,7 +4879,13 @@
         <v>363</v>
       </c>
     </row>
-    <row r="171" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>470</v>
+      </c>
+      <c r="B171" t="s">
+        <v>629</v>
+      </c>
       <c r="E171" t="s">
         <v>502</v>
       </c>
@@ -3837,7 +4893,13 @@
         <v>364</v>
       </c>
     </row>
-    <row r="172" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>471</v>
+      </c>
+      <c r="B172" t="s">
+        <v>630</v>
+      </c>
       <c r="E172" t="s">
         <v>503</v>
       </c>
@@ -3845,7 +4907,450 @@
         <v>365</v>
       </c>
     </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>472</v>
+      </c>
+      <c r="B173" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>473</v>
+      </c>
+      <c r="B174" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>474</v>
+      </c>
+      <c r="B175" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>475</v>
+      </c>
+      <c r="B176" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>476</v>
+      </c>
+      <c r="B177" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>477</v>
+      </c>
+      <c r="B178" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>478</v>
+      </c>
+      <c r="B179" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>479</v>
+      </c>
+      <c r="B180" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
+        <v>480</v>
+      </c>
+      <c r="B181" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
+        <v>481</v>
+      </c>
+      <c r="B182" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
+        <v>483</v>
+      </c>
+      <c r="B183" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
+        <v>484</v>
+      </c>
+      <c r="B184" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>485</v>
+      </c>
+      <c r="B185" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
+        <v>486</v>
+      </c>
+      <c r="B186" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
+        <v>487</v>
+      </c>
+      <c r="B187" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A188" t="s">
+        <v>489</v>
+      </c>
+      <c r="B188" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
+        <v>490</v>
+      </c>
+      <c r="B189" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A190" t="s">
+        <v>493</v>
+      </c>
+      <c r="B190" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
+        <v>494</v>
+      </c>
+      <c r="B191" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
+        <v>495</v>
+      </c>
+      <c r="B192" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>497</v>
+      </c>
+      <c r="B193" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>498</v>
+      </c>
+      <c r="B194" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A195" t="s">
+        <v>499</v>
+      </c>
+      <c r="B195" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>500</v>
+      </c>
+      <c r="B196" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
+        <v>503</v>
+      </c>
+      <c r="B197" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
+        <v>656</v>
+      </c>
+      <c r="B198" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A199" t="s">
+        <v>658</v>
+      </c>
+      <c r="B199" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
+        <v>660</v>
+      </c>
+      <c r="B200" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A201" t="s">
+        <v>662</v>
+      </c>
+      <c r="B201" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>664</v>
+      </c>
+      <c r="B202" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A203" t="s">
+        <v>665</v>
+      </c>
+      <c r="B203" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A204" t="s">
+        <v>667</v>
+      </c>
+      <c r="B204" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A205" t="s">
+        <v>669</v>
+      </c>
+      <c r="B205" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A206" t="s">
+        <v>670</v>
+      </c>
+      <c r="B206" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A207" t="s">
+        <v>672</v>
+      </c>
+      <c r="B207" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A208" t="s">
+        <v>674</v>
+      </c>
+      <c r="B208" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A209" t="s">
+        <v>676</v>
+      </c>
+      <c r="B209" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
+        <v>678</v>
+      </c>
+      <c r="B210" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
+        <v>680</v>
+      </c>
+      <c r="B211" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A212" t="s">
+        <v>682</v>
+      </c>
+      <c r="B212" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A213" t="s">
+        <v>684</v>
+      </c>
+      <c r="B213" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A214" t="s">
+        <v>686</v>
+      </c>
+      <c r="B214" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A215" t="s">
+        <v>688</v>
+      </c>
+      <c r="B215" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A216" t="s">
+        <v>690</v>
+      </c>
+      <c r="B216" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A217" t="s">
+        <v>692</v>
+      </c>
+      <c r="B217" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A218" t="s">
+        <v>694</v>
+      </c>
+      <c r="B218" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A219" t="s">
+        <v>696</v>
+      </c>
+      <c r="B219" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A220" t="s">
+        <v>698</v>
+      </c>
+      <c r="B220" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A221" t="s">
+        <v>700</v>
+      </c>
+      <c r="B221" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A222" t="s">
+        <v>702</v>
+      </c>
+      <c r="B222" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A223" t="s">
+        <v>704</v>
+      </c>
+      <c r="B223" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A224" t="s">
+        <v>706</v>
+      </c>
+      <c r="B224" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A225" t="s">
+        <v>708</v>
+      </c>
+      <c r="B225" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A226" t="s">
+        <v>710</v>
+      </c>
+      <c r="B226" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A227" t="s">
+        <v>712</v>
+      </c>
+      <c r="B227" t="s">
+        <v>713</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState ref="A2:B227">
+    <sortCondition ref="A2:A227"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>